<commit_message>
updated muscle grp data
</commit_message>
<xml_diff>
--- a/R/Included/Muscle_grp_data.xlsx
+++ b/R/Included/Muscle_grp_data.xlsx
@@ -5,20 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f01592f161d23204/Documents/GitHub/Systematic_lit_review/R/Included/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrf_g\Documents\GitHub\Systematic_lit_review\R\Included\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="13_ncr:1_{D0EAEB6E-E89C-4C60-AF3B-FE02DE16020F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1356BF9-5ABF-4A97-8B8D-FE82B0CA32A2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C28B815-1C6A-4215-94CA-21401F20A244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="1050" windowWidth="21060" windowHeight="16665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1395" yWindow="1050" windowWidth="32370" windowHeight="16665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ST muscles" sheetId="3" r:id="rId1"/>
-    <sheet name="reduced muscles" sheetId="1" r:id="rId2"/>
-    <sheet name="all muscles" sheetId="2" r:id="rId3"/>
+    <sheet name="Reduced" sheetId="4" r:id="rId2"/>
+    <sheet name="reduced muscles" sheetId="1" r:id="rId3"/>
+    <sheet name="all muscles" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'all muscles'!$A$1:$M$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'all muscles'!$A$1:$M$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="396">
   <si>
     <t>Muscle Name</t>
   </si>
@@ -1312,10 +1313,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1605,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6DAEAF-8D69-4940-9C0E-0B65ADDC6B11}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2893,11 +2890,446 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1A271D-20C9-4D5B-9FA7-9CA62C922F7D}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3701.5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>12.6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>63.4</v>
+      </c>
+      <c r="E2" s="3">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3">
+        <v>18.5</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3700</v>
+      </c>
+      <c r="C3" s="3">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="E3" s="3">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>364</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3692</v>
+      </c>
+      <c r="C4" s="3">
+        <v>13.966666666666667</v>
+      </c>
+      <c r="D4" s="3">
+        <v>63.800000000000004</v>
+      </c>
+      <c r="E4" s="3">
+        <v>17.333333333333332</v>
+      </c>
+      <c r="F4" s="3">
+        <v>18.833333333333332</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3713</v>
+      </c>
+      <c r="C5" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="F5" s="3">
+        <v>11.8</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>377</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3665</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10.7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="E6" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>380</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3663</v>
+      </c>
+      <c r="C7" s="3">
+        <v>13.4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>57.9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="F7" s="3">
+        <v>25.1</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3695.3333333333335</v>
+      </c>
+      <c r="C8" s="3">
+        <v>11.666666666666666</v>
+      </c>
+      <c r="D8" s="3">
+        <v>72.433333333333337</v>
+      </c>
+      <c r="E8" s="3">
+        <v>21.033333333333335</v>
+      </c>
+      <c r="F8" s="3">
+        <v>6.4666666666666659</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>351</v>
+      </c>
+      <c r="B9" s="3">
+        <v>3664</v>
+      </c>
+      <c r="C9" s="3">
+        <v>11.6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>55.55</v>
+      </c>
+      <c r="E9" s="3">
+        <v>25.5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>18.95</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>356</v>
+      </c>
+      <c r="B10" s="3">
+        <v>3693</v>
+      </c>
+      <c r="C10" s="3">
+        <v>11.7</v>
+      </c>
+      <c r="D10" s="3">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="E10" s="3">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="F10" s="3">
+        <v>13.9</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>359</v>
+      </c>
+      <c r="B11" s="3">
+        <v>3656</v>
+      </c>
+      <c r="C11" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45.5</v>
+      </c>
+      <c r="E11" s="3">
+        <v>32</v>
+      </c>
+      <c r="F11" s="3">
+        <v>22.5</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>360</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3677.8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>12.179999999999998</v>
+      </c>
+      <c r="D12" s="3">
+        <v>54.6</v>
+      </c>
+      <c r="E12" s="3">
+        <v>25.9</v>
+      </c>
+      <c r="F12" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>362</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3699.75</v>
+      </c>
+      <c r="C13" s="3">
+        <v>13.625</v>
+      </c>
+      <c r="D13" s="3">
+        <v>49.674999999999997</v>
+      </c>
+      <c r="E13" s="3">
+        <v>32.875</v>
+      </c>
+      <c r="F13" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>374</v>
+      </c>
+      <c r="B14" s="3">
+        <v>3702.6666666666665</v>
+      </c>
+      <c r="C14" s="3">
+        <v>12.199999999999998</v>
+      </c>
+      <c r="D14" s="3">
+        <v>45.300000000000004</v>
+      </c>
+      <c r="E14" s="3">
+        <v>33.966666666666669</v>
+      </c>
+      <c r="F14" s="3">
+        <v>20.766666666666666</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>333</v>
+      </c>
+      <c r="B15" s="3">
+        <v>3656</v>
+      </c>
+      <c r="C15" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="D15" s="3">
+        <v>53.45</v>
+      </c>
+      <c r="E15" s="3">
+        <v>30.85</v>
+      </c>
+      <c r="F15" s="3">
+        <v>15.7</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>366</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3671</v>
+      </c>
+      <c r="C16" s="3">
+        <v>13.3</v>
+      </c>
+      <c r="D16" s="3">
+        <v>52.8</v>
+      </c>
+      <c r="E16" s="3">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="F16" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>368</v>
+      </c>
+      <c r="B17" s="3">
+        <v>3623</v>
+      </c>
+      <c r="C17" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D17" s="3">
+        <v>63</v>
+      </c>
+      <c r="E17" s="3">
+        <v>25.3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>11.7</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>370</v>
+      </c>
+      <c r="B18" s="3">
+        <v>3662</v>
+      </c>
+      <c r="C18" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="D18" s="3">
+        <v>48.3</v>
+      </c>
+      <c r="E18" s="3">
+        <v>37.5</v>
+      </c>
+      <c r="F18" s="3">
+        <v>14.2</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>372</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3668</v>
+      </c>
+      <c r="C19" s="3">
+        <v>15.5</v>
+      </c>
+      <c r="D19" s="3">
+        <v>49.7</v>
+      </c>
+      <c r="E19" s="3">
+        <v>26.9</v>
+      </c>
+      <c r="F19" s="3">
+        <v>23.4</v>
+      </c>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>384</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3620</v>
+      </c>
+      <c r="C20" s="3">
+        <v>12</v>
+      </c>
+      <c r="D20" s="3">
+        <v>65.5</v>
+      </c>
+      <c r="E20" s="3">
+        <v>19</v>
+      </c>
+      <c r="F20" s="3">
+        <v>15.6</v>
+      </c>
+      <c r="G20" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3821,11 +4253,11 @@
         <v>3692</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" ref="G25:M25" si="4">AVERAGE(G22:G24)</f>
+        <f>AVERAGE(G22:G24)</f>
         <v>13.966666666666667</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="G25:M25" si="4">AVERAGE(H22:H24)</f>
         <v>63.800000000000004</v>
       </c>
       <c r="I25" s="2">
@@ -4719,12 +5151,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58846249-32A7-4BFC-BC49-CF1AF719CC3C}">
   <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>